<commit_message>
expanded for 25 points
can handle 25 data,
data must be full
</commit_message>
<xml_diff>
--- a/tsp.xlsx
+++ b/tsp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sameer\Documents\GitHub\tsp_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\tsp_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -360,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -505,17 +505,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -525,28 +514,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -597,7 +564,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,25 +575,10 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -984,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="A12:B13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,10 +972,12 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>2</v>
+        <f ca="1">RANDBETWEEN(-10,15)</f>
+        <v>-3</v>
+      </c>
+      <c r="B2" s="5">
+        <f ca="1">RANDBETWEEN(-10,15)</f>
+        <v>-9</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -1032,180 +986,348 @@
         <v>0</v>
       </c>
       <c r="J2" s="4">
-        <f>I3</f>
-        <v>1.5</v>
+        <f ca="1">I3</f>
+        <v>23</v>
       </c>
       <c r="K2" s="4">
-        <f>I4</f>
-        <v>5</v>
+        <f ca="1">I4</f>
+        <v>4</v>
       </c>
       <c r="L2" s="4">
-        <f>I5</f>
-        <v>4</v>
+        <f ca="1">I5</f>
+        <v>29</v>
       </c>
       <c r="M2" s="4">
-        <f>I6</f>
-        <v>5</v>
+        <f ca="1">I6</f>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8">
-        <v>2.5</v>
+      <c r="A3" s="5">
+        <f t="shared" ref="A3:B26" ca="1" si="0">RANDBETWEEN(-10,15)</f>
+        <v>-7</v>
+      </c>
+      <c r="B3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
       <c r="I3" s="4">
-        <f>ABS($A$2-A3)+ABS($B$2-B3)</f>
-        <v>1.5</v>
+        <f ca="1">ABS($A$2-A3)+ABS($B$2-B3)</f>
+        <v>23</v>
       </c>
       <c r="J3" s="4">
         <v>0</v>
       </c>
       <c r="K3" s="4">
-        <f>J4</f>
-        <v>3.5</v>
+        <f ca="1">J4</f>
+        <v>21</v>
       </c>
       <c r="L3" s="4">
-        <f>J5</f>
-        <v>4.5</v>
+        <f ca="1">J5</f>
+        <v>6</v>
       </c>
       <c r="M3" s="4">
-        <f>J6</f>
-        <v>5.5</v>
+        <f ca="1">J6</f>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8">
-        <v>5</v>
+      <c r="A4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="B4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-10</v>
       </c>
       <c r="H4" s="1">
         <v>2</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I6" si="0">ABS($A$2-A4)+ABS($B$2-B4)</f>
-        <v>5</v>
+        <f t="shared" ref="I4:I6" ca="1" si="1">ABS($A$2-A4)+ABS($B$2-B4)</f>
+        <v>4</v>
       </c>
       <c r="J4" s="4">
-        <f>ABS($A$3-A4)+ABS($B$3-B4)</f>
-        <v>3.5</v>
+        <f ca="1">ABS($A$3-A4)+ABS($B$3-B4)</f>
+        <v>21</v>
       </c>
       <c r="K4" s="4">
         <v>0</v>
       </c>
       <c r="L4" s="4">
-        <f>K5</f>
-        <v>7</v>
+        <f ca="1">K5</f>
+        <v>27</v>
       </c>
       <c r="M4" s="4">
-        <f>K6</f>
-        <v>4</v>
+        <f ca="1">K6</f>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>-2</v>
-      </c>
-      <c r="B5" s="8">
-        <v>3</v>
+      <c r="A5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="B5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>29</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J6" si="1">ABS($A$3-A5)+ABS($B$3-B5)</f>
-        <v>4.5</v>
+        <f t="shared" ref="J5:J6" ca="1" si="2">ABS($A$3-A5)+ABS($B$3-B5)</f>
+        <v>6</v>
       </c>
       <c r="K5" s="4">
-        <f>ABS($A$4-A5)+ABS($B$4-B5)</f>
-        <v>7</v>
+        <f ca="1">ABS($A$4-A5)+ABS($B$4-B5)</f>
+        <v>27</v>
       </c>
       <c r="L5" s="4">
         <v>0</v>
       </c>
       <c r="M5" s="4">
-        <f>L6</f>
-        <v>5</v>
+        <f ca="1">L6</f>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>0</v>
-      </c>
-      <c r="B6" s="10">
-        <v>6</v>
+      <c r="A6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="H6" s="1">
         <v>4</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
       </c>
       <c r="K6" s="4">
-        <f>ABS($A$4-A6)+ABS($B$4-B6)</f>
-        <v>4</v>
+        <f ca="1">ABS($A$4-A6)+ABS($B$4-B6)</f>
+        <v>40</v>
       </c>
       <c r="L6" s="4">
-        <f>ABS($A$5-A6)+ABS($B$5-B6)</f>
-        <v>5</v>
+        <f ca="1">ABS($A$5-A6)+ABS($B$5-B6)</f>
+        <v>23</v>
       </c>
       <c r="M6" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="B7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="B8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B18" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="B19" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="B20" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>-3.5</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="B21" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" ca="1" si="0"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>-2.5</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="B23" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" s="1">
-        <v>-2</v>
+      <c r="B24" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B25" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="B26" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>